<commit_message>
Pulo sintaxis, igualo bases y las pongo al principio de la serie.
</commit_message>
<xml_diff>
--- a/DATOS/RESULTADOS/ipc_inquilinos_estatal.xlsx
+++ b/DATOS/RESULTADOS/ipc_inquilinos_estatal.xlsx
@@ -399,13 +399,13 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>97.51272252350722</v>
+        <v>100</v>
       </c>
       <c r="D2" s="2">
         <v>43466</v>
       </c>
       <c r="E2">
-        <v>96.08499999999999</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -416,13 +416,13 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>97.69870314573896</v>
+        <v>100.1907244689911</v>
       </c>
       <c r="D3" s="2">
         <v>43497</v>
       </c>
       <c r="E3">
-        <v>96.31999999999999</v>
+        <v>100.2445751157829</v>
       </c>
     </row>
     <row r="4">
@@ -433,13 +433,13 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>98.20421998602659</v>
+        <v>100.7091356334069</v>
       </c>
       <c r="D4" s="2">
         <v>43525</v>
       </c>
       <c r="E4">
-        <v>96.669</v>
+        <v>100.6077951813499</v>
       </c>
     </row>
     <row r="5">
@@ -450,13 +450,13 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>99.21022586325735</v>
+        <v>101.7408019136589</v>
       </c>
       <c r="D5" s="2">
         <v>43556</v>
       </c>
       <c r="E5">
-        <v>97.64400000000001</v>
+        <v>101.6225217255555</v>
       </c>
     </row>
     <row r="6">
@@ -467,13 +467,13 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>99.58756543339153</v>
+        <v>102.1277663633934</v>
       </c>
       <c r="D6" s="2">
         <v>43586</v>
       </c>
       <c r="E6">
-        <v>97.834</v>
+        <v>101.8202633085289</v>
       </c>
     </row>
     <row r="7">
@@ -484,13 +484,13 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>99.71841607293898</v>
+        <v>102.2619546376628</v>
       </c>
       <c r="D7" s="2">
         <v>43617</v>
       </c>
       <c r="E7">
-        <v>97.71899999999999</v>
+        <v>101.7005776135713</v>
       </c>
     </row>
     <row r="8">
@@ -501,13 +501,13 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>99.22934341072109</v>
+        <v>101.7604070964176</v>
       </c>
       <c r="D8" s="2">
         <v>43647</v>
       </c>
       <c r="E8">
-        <v>97.113</v>
+        <v>101.0698860384035</v>
       </c>
     </row>
     <row r="9">
@@ -518,13 +518,13 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>99.18395602243879</v>
+        <v>101.7138620024979</v>
       </c>
       <c r="D9" s="2">
         <v>43678</v>
       </c>
       <c r="E9">
-        <v>97.059</v>
+        <v>101.0136857990321</v>
       </c>
     </row>
     <row r="10">
@@ -535,13 +535,13 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>98.95500188459366</v>
+        <v>101.4790678834126</v>
       </c>
       <c r="D10" s="2">
         <v>43709</v>
       </c>
       <c r="E10">
-        <v>97.059</v>
+        <v>101.0136857990321</v>
       </c>
     </row>
     <row r="11">
@@ -552,13 +552,13 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <v>99.48113949271229</v>
+        <v>102.0186257939117</v>
       </c>
       <c r="D11" s="2">
         <v>43739</v>
       </c>
       <c r="E11">
-        <v>98.001</v>
+        <v>101.9940677525108</v>
       </c>
     </row>
     <row r="12">
@@ -569,13 +569,13 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>99.83825399215294</v>
+        <v>102.3848492878302</v>
       </c>
       <c r="D12" s="2">
         <v>43770</v>
       </c>
       <c r="E12">
-        <v>98.167</v>
+        <v>102.1668314513192</v>
       </c>
     </row>
     <row r="13">
@@ -586,13 +586,13 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <v>100.0050260107236</v>
+        <v>102.5558751952757</v>
       </c>
       <c r="D13" s="2">
         <v>43800</v>
       </c>
       <c r="E13">
-        <v>98.096</v>
+        <v>102.0929385439975</v>
       </c>
     </row>
     <row r="14">
@@ -603,13 +603,13 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>99.23934757934764</v>
+        <v>101.7706664434727</v>
       </c>
       <c r="D14" s="2">
         <v>43831</v>
       </c>
       <c r="E14">
-        <v>97.139</v>
+        <v>101.0969454129156</v>
       </c>
     </row>
     <row r="15">
@@ -620,13 +620,13 @@
         <v>2</v>
       </c>
       <c r="C15">
-        <v>99.3796086926158</v>
+        <v>101.9145052263909</v>
       </c>
       <c r="D15" s="2">
         <v>43862</v>
       </c>
       <c r="E15">
-        <v>97.024</v>
+        <v>100.9772597179581</v>
       </c>
     </row>
     <row r="16">
@@ -637,13 +637,13 @@
         <v>3</v>
       </c>
       <c r="C16">
-        <v>99.31481018560939</v>
+        <v>101.8480538902683</v>
       </c>
       <c r="D16" s="2">
         <v>43891</v>
       </c>
       <c r="E16">
-        <v>96.652</v>
+        <v>100.5901025133996</v>
       </c>
     </row>
     <row r="17">
@@ -654,13 +654,13 @@
         <v>4</v>
       </c>
       <c r="C17">
-        <v>99.77996896572293</v>
+        <v>102.3250775729999</v>
       </c>
       <c r="D17" s="2">
         <v>43922</v>
       </c>
       <c r="E17">
-        <v>96.944</v>
+        <v>100.8940001040745</v>
       </c>
     </row>
     <row r="18">
@@ -671,13 +671,13 @@
         <v>5</v>
       </c>
       <c r="C18">
-        <v>100.0077876080712</v>
+        <v>102.5587072332664</v>
       </c>
       <c r="D18" s="2">
         <v>43952</v>
       </c>
       <c r="E18">
-        <v>96.938</v>
+        <v>100.8877556330333</v>
       </c>
     </row>
     <row r="19">
@@ -688,13 +688,13 @@
         <v>6</v>
       </c>
       <c r="C19">
-        <v>100.5948674333569</v>
+        <v>103.1607618268546</v>
       </c>
       <c r="D19" s="2">
         <v>43983</v>
       </c>
       <c r="E19">
-        <v>97.38500000000001</v>
+        <v>101.3529687256076</v>
       </c>
     </row>
     <row r="20">
@@ -705,13 +705,13 @@
         <v>7</v>
       </c>
       <c r="C20">
-        <v>99.89564115076296</v>
+        <v>102.4437002327376</v>
       </c>
       <c r="D20" s="2">
         <v>44013</v>
       </c>
       <c r="E20">
-        <v>96.511</v>
+        <v>100.4433574439298</v>
       </c>
     </row>
     <row r="21">
@@ -722,13 +722,13 @@
         <v>8</v>
       </c>
       <c r="C21">
-        <v>99.9294829530583</v>
+        <v>102.4784052449858</v>
       </c>
       <c r="D21" s="2">
         <v>44044</v>
       </c>
       <c r="E21">
-        <v>96.55500000000001</v>
+        <v>100.4891502315658</v>
       </c>
     </row>
     <row r="22">
@@ -739,13 +739,13 @@
         <v>9</v>
       </c>
       <c r="C22">
-        <v>99.80972244276765</v>
+        <v>102.3555899782274</v>
       </c>
       <c r="D22" s="2">
         <v>44075</v>
       </c>
       <c r="E22">
-        <v>96.7</v>
+        <v>100.6400582817297</v>
       </c>
     </row>
     <row r="23">
@@ -756,13 +756,13 @@
         <v>10</v>
       </c>
       <c r="C23">
-        <v>100.2130885795517</v>
+        <v>102.769244859709</v>
       </c>
       <c r="D23" s="2">
         <v>44105</v>
       </c>
       <c r="E23">
-        <v>97.208</v>
+        <v>101.1687568298902</v>
       </c>
     </row>
     <row r="24">
@@ -773,13 +773,13 @@
         <v>11</v>
       </c>
       <c r="C24">
-        <v>100.3388879102719</v>
+        <v>102.8982529803568</v>
       </c>
       <c r="D24" s="2">
         <v>44136</v>
       </c>
       <c r="E24">
-        <v>97.367</v>
+        <v>101.3342353124838</v>
       </c>
     </row>
     <row r="25">
@@ -790,13 +790,13 @@
         <v>12</v>
       </c>
       <c r="C25">
-        <v>100.2683904079147</v>
+        <v>102.8259572834132</v>
       </c>
       <c r="D25" s="2">
         <v>44166</v>
       </c>
       <c r="E25">
-        <v>97.574</v>
+        <v>101.5496695634074</v>
       </c>
     </row>
     <row r="26">
@@ -807,13 +807,13 @@
         <v>1</v>
       </c>
       <c r="C26">
-        <v>100</v>
+        <v>102.5507209850419</v>
       </c>
       <c r="D26" s="2">
         <v>44197</v>
       </c>
       <c r="E26">
-        <v>97.583</v>
+        <v>101.5590362699693</v>
       </c>
     </row>
     <row r="27">
@@ -824,13 +824,13 @@
         <v>2</v>
       </c>
       <c r="C27">
-        <v>99.29312052197895</v>
+        <v>101.825810983836</v>
       </c>
       <c r="D27" s="2">
         <v>44228</v>
       </c>
       <c r="E27">
-        <v>97.008</v>
+        <v>100.9606077951813</v>
       </c>
     </row>
     <row r="28">
@@ -841,13 +841,13 @@
         <v>3</v>
       </c>
       <c r="C28">
-        <v>99.99921286471898</v>
+        <v>102.5499137721361</v>
       </c>
       <c r="D28" s="2">
         <v>44256</v>
       </c>
       <c r="E28">
-        <v>97.949</v>
+        <v>101.9399490034865</v>
       </c>
     </row>
     <row r="29">
@@ -858,13 +858,13 @@
         <v>4</v>
       </c>
       <c r="C29">
-        <v>100.867268066879</v>
+        <v>103.4401106404993</v>
       </c>
       <c r="D29" s="2">
         <v>44287</v>
       </c>
       <c r="E29">
-        <v>99.105</v>
+        <v>103.1430504241037</v>
       </c>
     </row>
     <row r="30">
@@ -875,13 +875,13 @@
         <v>5</v>
       </c>
       <c r="C30">
-        <v>101.2169134424177</v>
+        <v>103.7986744940051</v>
       </c>
       <c r="D30" s="2">
         <v>44317</v>
       </c>
       <c r="E30">
-        <v>99.572</v>
+        <v>103.6290784201488</v>
       </c>
     </row>
     <row r="31">
@@ -892,13 +892,13 @@
         <v>6</v>
       </c>
       <c r="C31">
-        <v>101.5712489272691</v>
+        <v>104.1620480884261</v>
       </c>
       <c r="D31" s="2">
         <v>44348</v>
       </c>
       <c r="E31">
-        <v>100.046</v>
+        <v>104.1223916324088</v>
       </c>
     </row>
     <row r="32">
@@ -909,13 +909,13 @@
         <v>7</v>
       </c>
       <c r="C32">
-        <v>100.7300852772187</v>
+        <v>103.2994287006353</v>
       </c>
       <c r="D32" s="2">
         <v>44378</v>
       </c>
       <c r="E32">
-        <v>99.292</v>
+        <v>103.3376697715564</v>
       </c>
     </row>
     <row r="33">
@@ -926,13 +926,13 @@
         <v>8</v>
       </c>
       <c r="C33">
-        <v>101.0688688580645</v>
+        <v>103.6468537053716</v>
       </c>
       <c r="D33" s="2">
         <v>44409</v>
       </c>
       <c r="E33">
-        <v>99.74299999999999</v>
+        <v>103.8070458448249</v>
       </c>
     </row>
     <row r="34">
@@ -943,13 +943,13 @@
         <v>9</v>
       </c>
       <c r="C34">
-        <v>101.4193216989077</v>
+        <v>104.0062456203688</v>
       </c>
       <c r="D34" s="2">
         <v>44440</v>
       </c>
       <c r="E34">
-        <v>100.575</v>
+        <v>104.6729458292137</v>
       </c>
     </row>
     <row r="35">
@@ -960,13 +960,13 @@
         <v>10</v>
       </c>
       <c r="C35">
-        <v>102.8090123587009</v>
+        <v>105.4313834114486</v>
       </c>
       <c r="D35" s="2">
         <v>44470</v>
       </c>
       <c r="E35">
-        <v>102.425</v>
+        <v>106.5983244002706</v>
       </c>
     </row>
     <row r="36">
@@ -977,13 +977,13 @@
         <v>11</v>
       </c>
       <c r="C36">
-        <v>103.043258537902</v>
+        <v>105.6716045570993</v>
       </c>
       <c r="D36" s="2">
         <v>44501</v>
       </c>
       <c r="E36">
-        <v>102.738</v>
+        <v>106.92407763959</v>
       </c>
     </row>
     <row r="37">
@@ -994,13 +994,13 @@
         <v>12</v>
       </c>
       <c r="C37">
-        <v>103.9630198827306</v>
+        <v>106.6148264475627</v>
       </c>
       <c r="D37" s="2">
         <v>44531</v>
       </c>
       <c r="E37">
-        <v>103.965</v>
+        <v>108.2010719675287</v>
       </c>
     </row>
     <row r="38">
@@ -1011,13 +1011,13 @@
         <v>1</v>
       </c>
       <c r="C38">
-        <v>103.9540581538035</v>
+        <v>106.6056361299352</v>
       </c>
       <c r="D38" s="2">
         <v>44562</v>
       </c>
       <c r="E38">
-        <v>103.567</v>
+        <v>107.7868553884581</v>
       </c>
     </row>
     <row r="39">
@@ -1028,13 +1028,13 @@
         <v>2</v>
       </c>
       <c r="C39">
-        <v>104.5673225817185</v>
+        <v>107.2345432223069</v>
       </c>
       <c r="D39" s="2">
         <v>44593</v>
       </c>
       <c r="E39">
-        <v>104.403</v>
+        <v>108.6569183535411</v>
       </c>
     </row>
     <row r="40">
@@ -1045,13 +1045,13 @@
         <v>3</v>
       </c>
       <c r="C40">
-        <v>107.1860661179801</v>
+        <v>109.9200835994923</v>
       </c>
       <c r="D40" s="2">
         <v>44621</v>
       </c>
       <c r="E40">
-        <v>107.566</v>
+        <v>111.9487953374616</v>
       </c>
     </row>
     <row r="41">
@@ -1062,13 +1062,13 @@
         <v>4</v>
       </c>
       <c r="C41">
-        <v>107.0401595331048</v>
+        <v>109.770455344738</v>
       </c>
       <c r="D41" s="2">
         <v>44652</v>
       </c>
       <c r="E41">
-        <v>107.375</v>
+        <v>111.7500130093147</v>
       </c>
     </row>
     <row r="42">
@@ -1079,13 +1079,13 @@
         <v>5</v>
       </c>
       <c r="C42">
-        <v>107.9805007201712</v>
+        <v>110.7347820117939</v>
       </c>
       <c r="D42" s="2">
         <v>44682</v>
       </c>
       <c r="E42">
-        <v>108.262</v>
+        <v>112.6731539782484</v>
       </c>
     </row>
     <row r="43">
@@ -1096,13 +1096,13 @@
         <v>6</v>
       </c>
       <c r="C43">
-        <v>110.0351653806988</v>
+        <v>112.8418554349898</v>
       </c>
       <c r="D43" s="2">
         <v>44713</v>
       </c>
       <c r="E43">
-        <v>110.267</v>
+        <v>114.7598480512047</v>
       </c>
     </row>
     <row r="44">
@@ -1113,13 +1113,13 @@
         <v>7</v>
       </c>
       <c r="C44">
-        <v>110.113382810351</v>
+        <v>112.9220679730341</v>
       </c>
       <c r="D44" s="2">
         <v>44743</v>
       </c>
       <c r="E44">
-        <v>109.986</v>
+        <v>114.4673986574387</v>
       </c>
     </row>
     <row r="45">
@@ -1130,13 +1130,13 @@
         <v>8</v>
       </c>
       <c r="C45">
-        <v>110.3167133881492</v>
+        <v>113.1305849465492</v>
       </c>
       <c r="D45" s="2">
         <v>44774</v>
       </c>
       <c r="E45">
-        <v>110.265</v>
+        <v>114.7577665608576</v>
       </c>
     </row>
     <row r="46">
@@ -1147,13 +1147,13 @@
         <v>9</v>
       </c>
       <c r="C46">
-        <v>109.4584115422884</v>
+        <v>112.2503902153911</v>
       </c>
       <c r="D46" s="2">
         <v>44805</v>
       </c>
       <c r="E46">
-        <v>109.498</v>
+        <v>113.9595150127492</v>
       </c>
     </row>
     <row r="47">
@@ -1164,13 +1164,13 @@
         <v>10</v>
       </c>
       <c r="C47">
-        <v>109.7258314331384</v>
+        <v>112.5246312415151</v>
       </c>
       <c r="D47" s="2">
         <v>44835</v>
       </c>
       <c r="E47">
-        <v>109.866</v>
+        <v>114.3425092366134</v>
       </c>
     </row>
     <row r="48">
@@ -1181,13 +1181,13 @@
         <v>11</v>
       </c>
       <c r="C48">
-        <v>109.9134098877834</v>
+        <v>112.7169942991662</v>
       </c>
       <c r="D48" s="2">
         <v>44866</v>
       </c>
       <c r="E48">
-        <v>109.734</v>
+        <v>114.2051308737056</v>
       </c>
     </row>
     <row r="49">
@@ -1198,13 +1198,13 @@
         <v>12</v>
       </c>
       <c r="C49">
-        <v>110.3197463891681</v>
+        <v>113.1336953109616</v>
       </c>
       <c r="D49" s="2">
         <v>44896</v>
       </c>
       <c r="E49">
-        <v>109.899</v>
+        <v>114.3768538273404</v>
       </c>
     </row>
     <row r="50">
@@ -1215,13 +1215,13 @@
         <v>1</v>
       </c>
       <c r="C50">
-        <v>110.6827680711938</v>
+        <v>113.505976663211</v>
       </c>
       <c r="D50" s="2">
         <v>44927</v>
       </c>
       <c r="E50">
-        <v>109.668</v>
+        <v>114.1364416922517</v>
       </c>
     </row>
     <row r="51">
@@ -1232,13 +1232,13 @@
         <v>2</v>
       </c>
       <c r="C51">
-        <v>111.4613489996468</v>
+        <v>114.3044170187916</v>
       </c>
       <c r="D51" s="2">
         <v>44958</v>
       </c>
       <c r="E51">
-        <v>110.703</v>
+        <v>115.21361294687</v>
       </c>
     </row>
     <row r="52">
@@ -1249,13 +1249,13 @@
         <v>3</v>
       </c>
       <c r="C52">
-        <v>112.0354998306003</v>
+        <v>114.893212835476</v>
       </c>
       <c r="D52" s="2">
         <v>44986</v>
       </c>
       <c r="E52">
-        <v>111.111</v>
+        <v>115.638236977676</v>
       </c>
     </row>
     <row r="53">
@@ -1266,13 +1266,13 @@
         <v>4</v>
       </c>
       <c r="C53">
-        <v>113.0765161999174</v>
+        <v>115.960782627783</v>
       </c>
       <c r="D53" s="2">
         <v>45017</v>
       </c>
       <c r="E53">
-        <v>111.773</v>
+        <v>116.3272102825623</v>
       </c>
     </row>
     <row r="54">
@@ -1283,13 +1283,13 @@
         <v>5</v>
       </c>
       <c r="C54">
-        <v>113.3019597943043</v>
+        <v>116.1919766592413</v>
       </c>
       <c r="D54" s="2">
         <v>45047</v>
       </c>
       <c r="E54">
-        <v>111.719</v>
+        <v>116.2710100431909</v>
       </c>
     </row>
     <row r="55">
@@ -1300,13 +1300,13 @@
         <v>6</v>
       </c>
       <c r="C55">
-        <v>114.3246246435287</v>
+        <v>117.2407268353815</v>
       </c>
       <c r="D55" s="2">
         <v>45078</v>
       </c>
       <c r="E55">
-        <v>112.354</v>
+        <v>116.9318832283915</v>
       </c>
     </row>
     <row r="56">
@@ -1317,13 +1317,13 @@
         <v>7</v>
       </c>
       <c r="C56">
-        <v>114.7360872220881</v>
+        <v>117.6626846762779</v>
       </c>
       <c r="D56" s="2">
         <v>45108</v>
       </c>
       <c r="E56">
-        <v>112.544</v>
+        <v>117.1296248113649</v>
       </c>
     </row>
     <row r="57">
@@ -1334,13 +1334,13 @@
         <v>8</v>
       </c>
       <c r="C57">
-        <v>115.1926143345042</v>
+        <v>118.1308565215528</v>
       </c>
       <c r="D57" s="2">
         <v>45139</v>
       </c>
       <c r="E57">
-        <v>113.149</v>
+        <v>117.7592756413592</v>
       </c>
     </row>
     <row r="58">
@@ -1351,13 +1351,13 @@
         <v>9</v>
       </c>
       <c r="C58">
-        <v>115.0672168681821</v>
+        <v>118.0022605157424</v>
       </c>
       <c r="D58" s="2">
         <v>45170</v>
       </c>
       <c r="E58">
-        <v>113.348</v>
+        <v>117.9663839308945</v>
       </c>
     </row>
     <row r="59">
@@ -1368,13 +1368,13 @@
         <v>10</v>
       </c>
       <c r="C59">
-        <v>115.3115288725653</v>
+        <v>118.2528042376905</v>
       </c>
       <c r="D59" s="2">
         <v>45200</v>
       </c>
       <c r="E59">
-        <v>113.676</v>
+        <v>118.3077483478171</v>
       </c>
     </row>
     <row r="60">
@@ -1385,13 +1385,13 @@
         <v>11</v>
       </c>
       <c r="C60">
-        <v>115.2780050377524</v>
+        <v>118.218425303388</v>
       </c>
       <c r="D60" s="2">
         <v>45231</v>
       </c>
       <c r="E60">
-        <v>113.28</v>
+        <v>117.8956132590935</v>
       </c>
     </row>
     <row r="61">
@@ -1402,13 +1402,13 @@
         <v>12</v>
       </c>
       <c r="C61">
-        <v>115.8405155885507</v>
+        <v>118.7952839288486</v>
       </c>
       <c r="D61" s="2">
         <v>45261</v>
       </c>
       <c r="E61">
-        <v>113.308</v>
+        <v>117.9247541239528</v>
       </c>
     </row>
     <row r="62">
@@ -1419,13 +1419,13 @@
         <v>1</v>
       </c>
       <c r="C62">
-        <v>116.6852303540751</v>
+        <v>119.661545011161</v>
       </c>
       <c r="D62" s="2">
         <v>45292</v>
       </c>
       <c r="E62">
-        <v>113.404</v>
+        <v>118.024665660613</v>
       </c>
     </row>
     <row r="63">
@@ -1436,13 +1436,13 @@
         <v>2</v>
       </c>
       <c r="C63">
-        <v>117.5066334531552</v>
+        <v>120.503899811461</v>
       </c>
       <c r="D63" s="2">
         <v>45323</v>
       </c>
       <c r="E63">
-        <v>113.807</v>
+        <v>118.4440859655513</v>
       </c>
     </row>
     <row r="64">
@@ -1453,13 +1453,13 @@
         <v>3</v>
       </c>
       <c r="C64">
-        <v>118.4273243608429</v>
+        <v>121.4480749753385</v>
       </c>
       <c r="D64" s="2">
         <v>45352</v>
       </c>
       <c r="E64">
-        <v>114.674</v>
+        <v>119.3464120310142</v>
       </c>
     </row>
     <row r="65">
@@ -1470,13 +1470,13 @@
         <v>4</v>
       </c>
       <c r="C65">
-        <v>119.0361152343294</v>
+        <v>122.0723944053901</v>
       </c>
       <c r="D65" s="2">
         <v>45383</v>
       </c>
       <c r="E65">
-        <v>115.472</v>
+        <v>120.1769266795025</v>
       </c>
     </row>
     <row r="66">
@@ -1487,13 +1487,13 @@
         <v>5</v>
       </c>
       <c r="C66">
-        <v>120.5573651314358</v>
+        <v>123.6324471428569</v>
       </c>
       <c r="D66" s="2">
         <v>45413</v>
       </c>
       <c r="E66">
-        <v>115.776</v>
+        <v>120.49331321226</v>
       </c>
     </row>
     <row r="67">
@@ -1504,13 +1504,13 @@
         <v>6</v>
       </c>
       <c r="C67">
-        <v>121.4065790342464</v>
+        <v>124.5033221228943</v>
       </c>
       <c r="D67" s="2">
         <v>45444</v>
       </c>
       <c r="E67">
-        <v>116.212</v>
+        <v>120.9470781079253</v>
       </c>
     </row>
     <row r="68">
@@ -1521,13 +1521,13 @@
         <v>7</v>
       </c>
       <c r="C68">
-        <v>120.1997202968823</v>
+        <v>123.2656797864565</v>
       </c>
       <c r="D68" s="2">
         <v>45474</v>
       </c>
       <c r="E68">
-        <v>115.66</v>
+        <v>120.3725867721289</v>
       </c>
     </row>
     <row r="69">
@@ -1538,13 +1538,13 @@
         <v>8</v>
       </c>
       <c r="C69">
-        <v>120.2320000179186</v>
+        <v>123.2987828731112</v>
       </c>
       <c r="D69" s="2">
         <v>45505</v>
       </c>
       <c r="E69">
-        <v>115.707</v>
+        <v>120.4215017952854</v>
       </c>
     </row>
     <row r="70">
@@ -1555,13 +1555,13 @@
         <v>9</v>
       </c>
       <c r="C70">
-        <v>119.4286429273413</v>
+        <v>122.4749343846397</v>
       </c>
       <c r="D70" s="2">
         <v>45536</v>
       </c>
       <c r="E70">
-        <v>115.009</v>
+        <v>119.6950616641515</v>
       </c>
     </row>
     <row r="71">
@@ -1572,13 +1572,13 @@
         <v>10</v>
       </c>
       <c r="C71">
-        <v>119.9761507821712</v>
+        <v>123.0364076372175</v>
       </c>
       <c r="D71" s="2">
         <v>45566</v>
       </c>
       <c r="E71">
-        <v>115.726</v>
+        <v>120.4412759535828</v>
       </c>
     </row>
     <row r="72">
@@ -1589,13 +1589,13 @@
         <v>11</v>
       </c>
       <c r="C72">
-        <v>120.9647688835819</v>
+        <v>124.0502426280028</v>
       </c>
       <c r="D72" s="2">
         <v>45597</v>
       </c>
       <c r="E72">
-        <v>116.01</v>
+        <v>120.7368475828694</v>
       </c>
     </row>
     <row r="73">
@@ -1606,13 +1606,13 @@
         <v>12</v>
       </c>
       <c r="C73">
-        <v>121.8831692078534</v>
+        <v>124.9920687820722</v>
       </c>
       <c r="D73" s="2">
         <v>45627</v>
       </c>
       <c r="E73">
-        <v>116.534</v>
+        <v>121.2821980538065</v>
       </c>
     </row>
     <row r="74">
@@ -1623,13 +1623,13 @@
         <v>1</v>
       </c>
       <c r="C74">
-        <v>122.7084576593252</v>
+        <v>125.8384080392628</v>
       </c>
       <c r="D74" s="2">
         <v>45658</v>
       </c>
       <c r="E74">
-        <v>116.733</v>
+        <v>121.4893063433419</v>
       </c>
     </row>
     <row r="75">
@@ -1640,13 +1640,13 @@
         <v>2</v>
       </c>
       <c r="C75">
-        <v>123.519749170043</v>
+        <v>126.6703933327943</v>
       </c>
       <c r="D75" s="2">
         <v>45689</v>
       </c>
       <c r="E75">
-        <v>117.191</v>
+        <v>121.9659676328251</v>
       </c>
     </row>
     <row r="76">
@@ -1657,13 +1657,13 @@
         <v>3</v>
       </c>
       <c r="C76">
-        <v>123.567313132901</v>
+        <v>126.7191705196343</v>
       </c>
       <c r="D76" s="2">
         <v>45717</v>
       </c>
       <c r="E76">
-        <v>117.26</v>
+        <v>122.0377790497997</v>
       </c>
     </row>
     <row r="77">
@@ -1674,13 +1674,13 @@
         <v>4</v>
       </c>
       <c r="C77">
-        <v>124.8284044731425</v>
+        <v>128.0124287813319</v>
       </c>
       <c r="D77" s="2">
         <v>45748</v>
       </c>
       <c r="E77">
-        <v>117.997</v>
+        <v>122.8048082427018</v>
       </c>
     </row>
     <row r="78">
@@ -1691,13 +1691,13 @@
         <v>5</v>
       </c>
       <c r="C78">
-        <v>125.3330465733894</v>
+        <v>128.5299428935291</v>
       </c>
       <c r="D78" s="2">
         <v>45778</v>
       </c>
       <c r="E78">
-        <v>118.077</v>
+        <v>122.8880678565853</v>
       </c>
     </row>
     <row r="79">
@@ -1708,13 +1708,13 @@
         <v>6</v>
       </c>
       <c r="C79">
-        <v>126.1936909529623</v>
+        <v>129.4125399098983</v>
       </c>
       <c r="D79" s="2">
         <v>45809</v>
       </c>
       <c r="E79">
-        <v>118.867</v>
+        <v>123.7102565436853</v>
       </c>
     </row>
     <row r="80">
@@ -1725,13 +1725,13 @@
         <v>7</v>
       </c>
       <c r="C80">
-        <v>126.1149877939172</v>
+        <v>129.3318292528596</v>
       </c>
       <c r="D80" s="2">
         <v>45839</v>
       </c>
       <c r="E80">
-        <v>118.777</v>
+        <v>123.6165894780663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Miro de calcular medias anuales, en proceso
</commit_message>
<xml_diff>
--- a/DATOS/RESULTADOS/ipc_inquilinos_estatal.xlsx
+++ b/DATOS/RESULTADOS/ipc_inquilinos_estatal.xlsx
@@ -1,24 +1,50 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lorie\Desktop\TRABAJO\CGT\Análisis de coyuntura económica\IPC\Nuevo calculo de IPC alternativo para inquilinos\reponderacionIPC_2\DATOS\RESULTADOS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>anio</t>
+  </si>
+  <si>
+    <t>mes</t>
+  </si>
+  <si>
+    <t>ipc_inquilinos</t>
+  </si>
+  <si>
+    <t>fecha</t>
+  </si>
+  <si>
+    <t>ipc_oficial</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,6 +54,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -52,26 +85,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -113,7 +157,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -145,9 +189,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -179,6 +224,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -354,44 +400,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E85"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="J82" sqref="J82"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="20.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>anio</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>mes</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>ipc_inquilinos</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>fecha</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>ipc_oficial</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -408,7 +446,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -416,16 +454,16 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>100.1907244689911</v>
+        <v>100.19072446899111</v>
       </c>
       <c r="D3" s="2">
         <v>43497</v>
       </c>
       <c r="E3">
-        <v>100.2445751157829</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>100.24457511578289</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2019</v>
       </c>
@@ -442,7 +480,7 @@
         <v>100.6077951813499</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2019</v>
       </c>
@@ -459,7 +497,7 @@
         <v>101.6225217255555</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2019</v>
       </c>
@@ -467,16 +505,16 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>102.1277663633934</v>
+        <v>102.12776636339341</v>
       </c>
       <c r="D6" s="2">
         <v>43586</v>
       </c>
       <c r="E6">
-        <v>101.8202633085289</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>101.82026330852889</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2019</v>
       </c>
@@ -493,7 +531,7 @@
         <v>101.7005776135713</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2019</v>
       </c>
@@ -501,7 +539,7 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>101.7604070964176</v>
+        <v>101.76040709641759</v>
       </c>
       <c r="D8" s="2">
         <v>43647</v>
@@ -510,7 +548,7 @@
         <v>101.0698860384035</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2019</v>
       </c>
@@ -527,7 +565,7 @@
         <v>101.0136857990321</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2019</v>
       </c>
@@ -544,7 +582,7 @@
         <v>101.0136857990321</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2019</v>
       </c>
@@ -561,7 +599,7 @@
         <v>101.9940677525108</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2019</v>
       </c>
@@ -569,7 +607,7 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>102.3848492878302</v>
+        <v>102.38484928783021</v>
       </c>
       <c r="D12" s="2">
         <v>43770</v>
@@ -578,7 +616,7 @@
         <v>102.1668314513192</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2019</v>
       </c>
@@ -592,10 +630,10 @@
         <v>43800</v>
       </c>
       <c r="E13">
-        <v>102.0929385439975</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>102.09293854399751</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2020</v>
       </c>
@@ -603,7 +641,7 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>101.7706664434727</v>
+        <v>101.77066644347271</v>
       </c>
       <c r="D14" s="2">
         <v>43831</v>
@@ -612,7 +650,7 @@
         <v>101.0969454129156</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2020</v>
       </c>
@@ -626,10 +664,10 @@
         <v>43862</v>
       </c>
       <c r="E15">
-        <v>100.9772597179581</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>100.97725971795811</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2020</v>
       </c>
@@ -646,7 +684,7 @@
         <v>100.5901025133996</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2020</v>
       </c>
@@ -660,10 +698,10 @@
         <v>43922</v>
       </c>
       <c r="E17">
-        <v>100.8940001040745</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>100.89400010407449</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2020</v>
       </c>
@@ -677,10 +715,10 @@
         <v>43952</v>
       </c>
       <c r="E18">
-        <v>100.8877556330333</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>100.88775563303329</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2020</v>
       </c>
@@ -697,7 +735,7 @@
         <v>101.3529687256076</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2020</v>
       </c>
@@ -714,7 +752,7 @@
         <v>100.4433574439298</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2020</v>
       </c>
@@ -722,7 +760,7 @@
         <v>8</v>
       </c>
       <c r="C21">
-        <v>102.4784052449858</v>
+        <v>102.47840524498579</v>
       </c>
       <c r="D21" s="2">
         <v>44044</v>
@@ -731,7 +769,7 @@
         <v>100.4891502315658</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2020</v>
       </c>
@@ -745,10 +783,10 @@
         <v>44075</v>
       </c>
       <c r="E22">
-        <v>100.6400582817297</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>100.64005828172969</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2020</v>
       </c>
@@ -765,7 +803,7 @@
         <v>101.1687568298902</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2020</v>
       </c>
@@ -782,7 +820,7 @@
         <v>101.3342353124838</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2020</v>
       </c>
@@ -796,10 +834,10 @@
         <v>44166</v>
       </c>
       <c r="E25">
-        <v>101.5496695634074</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>101.54966956340741</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2021</v>
       </c>
@@ -807,7 +845,7 @@
         <v>1</v>
       </c>
       <c r="C26">
-        <v>102.5507209850419</v>
+        <v>102.55072098504191</v>
       </c>
       <c r="D26" s="2">
         <v>44197</v>
@@ -816,7 +854,7 @@
         <v>101.5590362699693</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2021</v>
       </c>
@@ -824,7 +862,7 @@
         <v>2</v>
       </c>
       <c r="C27">
-        <v>101.825810983836</v>
+        <v>101.82581098383601</v>
       </c>
       <c r="D27" s="2">
         <v>44228</v>
@@ -833,7 +871,7 @@
         <v>100.9606077951813</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2021</v>
       </c>
@@ -841,7 +879,7 @@
         <v>3</v>
       </c>
       <c r="C28">
-        <v>102.5499137721361</v>
+        <v>102.54991377213609</v>
       </c>
       <c r="D28" s="2">
         <v>44256</v>
@@ -850,7 +888,7 @@
         <v>101.9399490034865</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2021</v>
       </c>
@@ -864,10 +902,10 @@
         <v>44287</v>
       </c>
       <c r="E29">
-        <v>103.1430504241037</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>103.14305042410371</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2021</v>
       </c>
@@ -884,7 +922,7 @@
         <v>103.6290784201488</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2021</v>
       </c>
@@ -898,10 +936,10 @@
         <v>44348</v>
       </c>
       <c r="E31">
-        <v>104.1223916324088</v>
-      </c>
-    </row>
-    <row r="32">
+        <v>104.12239163240881</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2021</v>
       </c>
@@ -915,10 +953,10 @@
         <v>44378</v>
       </c>
       <c r="E32">
-        <v>103.3376697715564</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>103.33766977155641</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2021</v>
       </c>
@@ -935,7 +973,7 @@
         <v>103.8070458448249</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2021</v>
       </c>
@@ -952,7 +990,7 @@
         <v>104.6729458292137</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2021</v>
       </c>
@@ -960,7 +998,7 @@
         <v>10</v>
       </c>
       <c r="C35">
-        <v>105.4313834114486</v>
+        <v>105.43138341144861</v>
       </c>
       <c r="D35" s="2">
         <v>44470</v>
@@ -969,7 +1007,7 @@
         <v>106.5983244002706</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2021</v>
       </c>
@@ -986,7 +1024,7 @@
         <v>106.92407763959</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2021</v>
       </c>
@@ -994,7 +1032,7 @@
         <v>12</v>
       </c>
       <c r="C37">
-        <v>106.6148264475627</v>
+        <v>106.61482644756271</v>
       </c>
       <c r="D37" s="2">
         <v>44531</v>
@@ -1003,7 +1041,7 @@
         <v>108.2010719675287</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2022</v>
       </c>
@@ -1011,16 +1049,16 @@
         <v>1</v>
       </c>
       <c r="C38">
-        <v>106.6056361299352</v>
+        <v>106.60563612993521</v>
       </c>
       <c r="D38" s="2">
         <v>44562</v>
       </c>
       <c r="E38">
-        <v>107.7868553884581</v>
-      </c>
-    </row>
-    <row r="39">
+        <v>107.78685538845809</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2022</v>
       </c>
@@ -1037,7 +1075,7 @@
         <v>108.6569183535411</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2022</v>
       </c>
@@ -1054,7 +1092,7 @@
         <v>111.9487953374616</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2022</v>
       </c>
@@ -1071,7 +1109,7 @@
         <v>111.7500130093147</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2022</v>
       </c>
@@ -1085,10 +1123,10 @@
         <v>44682</v>
       </c>
       <c r="E42">
-        <v>112.6731539782484</v>
-      </c>
-    </row>
-    <row r="43">
+        <v>112.67315397824839</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2022</v>
       </c>
@@ -1105,7 +1143,7 @@
         <v>114.7598480512047</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2022</v>
       </c>
@@ -1119,10 +1157,10 @@
         <v>44743</v>
       </c>
       <c r="E44">
-        <v>114.4673986574387</v>
-      </c>
-    </row>
-    <row r="45">
+        <v>114.46739865743869</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2022</v>
       </c>
@@ -1130,7 +1168,7 @@
         <v>8</v>
       </c>
       <c r="C45">
-        <v>113.1305849465492</v>
+        <v>113.13058494654921</v>
       </c>
       <c r="D45" s="2">
         <v>44774</v>
@@ -1139,7 +1177,7 @@
         <v>114.7577665608576</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2022</v>
       </c>
@@ -1147,16 +1185,16 @@
         <v>9</v>
       </c>
       <c r="C46">
-        <v>112.2503902153911</v>
+        <v>112.25039021539111</v>
       </c>
       <c r="D46" s="2">
         <v>44805</v>
       </c>
       <c r="E46">
-        <v>113.9595150127492</v>
-      </c>
-    </row>
-    <row r="47">
+        <v>113.95951501274919</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2022</v>
       </c>
@@ -1173,7 +1211,7 @@
         <v>114.3425092366134</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2022</v>
       </c>
@@ -1190,7 +1228,7 @@
         <v>114.2051308737056</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2022</v>
       </c>
@@ -1207,7 +1245,7 @@
         <v>114.3768538273404</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2023</v>
       </c>
@@ -1221,10 +1259,10 @@
         <v>44927</v>
       </c>
       <c r="E50">
-        <v>114.1364416922517</v>
-      </c>
-    </row>
-    <row r="51">
+        <v>114.13644169225169</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2023</v>
       </c>
@@ -1241,7 +1279,7 @@
         <v>115.21361294687</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2023</v>
       </c>
@@ -1249,7 +1287,7 @@
         <v>3</v>
       </c>
       <c r="C52">
-        <v>114.893212835476</v>
+        <v>114.89321283547601</v>
       </c>
       <c r="D52" s="2">
         <v>44986</v>
@@ -1258,7 +1296,7 @@
         <v>115.638236977676</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2023</v>
       </c>
@@ -1272,10 +1310,10 @@
         <v>45017</v>
       </c>
       <c r="E53">
-        <v>116.3272102825623</v>
-      </c>
-    </row>
-    <row r="54">
+        <v>116.32721028256231</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2023</v>
       </c>
@@ -1283,7 +1321,7 @@
         <v>5</v>
       </c>
       <c r="C54">
-        <v>116.1919766592413</v>
+        <v>116.19197665924131</v>
       </c>
       <c r="D54" s="2">
         <v>45047</v>
@@ -1292,7 +1330,7 @@
         <v>116.2710100431909</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2023</v>
       </c>
@@ -1300,7 +1338,7 @@
         <v>6</v>
       </c>
       <c r="C55">
-        <v>117.2407268353815</v>
+        <v>117.24072683538149</v>
       </c>
       <c r="D55" s="2">
         <v>45078</v>
@@ -1309,7 +1347,7 @@
         <v>116.9318832283915</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2023</v>
       </c>
@@ -1317,16 +1355,16 @@
         <v>7</v>
       </c>
       <c r="C56">
-        <v>117.6626846762779</v>
+        <v>117.66268467627791</v>
       </c>
       <c r="D56" s="2">
         <v>45108</v>
       </c>
       <c r="E56">
-        <v>117.1296248113649</v>
-      </c>
-    </row>
-    <row r="57">
+        <v>117.12962481136491</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2023</v>
       </c>
@@ -1343,7 +1381,7 @@
         <v>117.7592756413592</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2023</v>
       </c>
@@ -1351,16 +1389,16 @@
         <v>9</v>
       </c>
       <c r="C58">
-        <v>118.0022605157424</v>
+        <v>118.00226051574241</v>
       </c>
       <c r="D58" s="2">
         <v>45170</v>
       </c>
       <c r="E58">
-        <v>117.9663839308945</v>
-      </c>
-    </row>
-    <row r="59">
+        <v>117.96638393089449</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2023</v>
       </c>
@@ -1377,7 +1415,7 @@
         <v>118.3077483478171</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2023</v>
       </c>
@@ -1391,10 +1429,10 @@
         <v>45231</v>
       </c>
       <c r="E60">
-        <v>117.8956132590935</v>
-      </c>
-    </row>
-    <row r="61">
+        <v>117.89561325909349</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2023</v>
       </c>
@@ -1408,10 +1446,10 @@
         <v>45261</v>
       </c>
       <c r="E61">
-        <v>117.9247541239528</v>
-      </c>
-    </row>
-    <row r="62">
+        <v>117.92475412395279</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2024</v>
       </c>
@@ -1428,7 +1466,7 @@
         <v>118.024665660613</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2024</v>
       </c>
@@ -1445,7 +1483,7 @@
         <v>118.4440859655513</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>2024</v>
       </c>
@@ -1462,7 +1500,7 @@
         <v>119.3464120310142</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>2024</v>
       </c>
@@ -1479,7 +1517,7 @@
         <v>120.1769266795025</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2024</v>
       </c>
@@ -1493,10 +1531,10 @@
         <v>45413</v>
       </c>
       <c r="E66">
-        <v>120.49331321226</v>
-      </c>
-    </row>
-    <row r="67">
+        <v>120.49331321226001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>2024</v>
       </c>
@@ -1510,10 +1548,10 @@
         <v>45444</v>
       </c>
       <c r="E67">
-        <v>120.9470781079253</v>
-      </c>
-    </row>
-    <row r="68">
+        <v>120.94707810792529</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>2024</v>
       </c>
@@ -1530,7 +1568,7 @@
         <v>120.3725867721289</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>2024</v>
       </c>
@@ -1538,16 +1576,16 @@
         <v>8</v>
       </c>
       <c r="C69">
-        <v>123.2987828731112</v>
+        <v>123.29878287311119</v>
       </c>
       <c r="D69" s="2">
         <v>45505</v>
       </c>
       <c r="E69">
-        <v>120.4215017952854</v>
-      </c>
-    </row>
-    <row r="70">
+        <v>120.42150179528539</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>2024</v>
       </c>
@@ -1564,7 +1602,7 @@
         <v>119.6950616641515</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>2024</v>
       </c>
@@ -1572,7 +1610,7 @@
         <v>10</v>
       </c>
       <c r="C71">
-        <v>123.0364076372175</v>
+        <v>123.03640763721749</v>
       </c>
       <c r="D71" s="2">
         <v>45566</v>
@@ -1581,7 +1619,7 @@
         <v>120.4412759535828</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>2024</v>
       </c>
@@ -1589,7 +1627,7 @@
         <v>11</v>
       </c>
       <c r="C72">
-        <v>124.0502426280028</v>
+        <v>124.05024262800281</v>
       </c>
       <c r="D72" s="2">
         <v>45597</v>
@@ -1598,7 +1636,7 @@
         <v>120.7368475828694</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>2024</v>
       </c>
@@ -1615,7 +1653,7 @@
         <v>121.2821980538065</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>2025</v>
       </c>
@@ -1629,10 +1667,10 @@
         <v>45658</v>
       </c>
       <c r="E74">
-        <v>121.4893063433419</v>
-      </c>
-    </row>
-    <row r="75">
+        <v>121.48930634334189</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>2025</v>
       </c>
@@ -1649,7 +1687,7 @@
         <v>121.9659676328251</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>2025</v>
       </c>
@@ -1666,7 +1704,7 @@
         <v>122.0377790497997</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>2025</v>
       </c>
@@ -1674,7 +1712,7 @@
         <v>4</v>
       </c>
       <c r="C77">
-        <v>128.0124287813319</v>
+        <v>128.01242878133189</v>
       </c>
       <c r="D77" s="2">
         <v>45748</v>
@@ -1683,7 +1721,7 @@
         <v>122.8048082427018</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>2025</v>
       </c>
@@ -1697,10 +1735,10 @@
         <v>45778</v>
       </c>
       <c r="E78">
-        <v>122.8880678565853</v>
-      </c>
-    </row>
-    <row r="79">
+        <v>122.88806785658529</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>2025</v>
       </c>
@@ -1717,7 +1755,7 @@
         <v>123.7102565436853</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>2025</v>
       </c>
@@ -1725,7 +1763,7 @@
         <v>7</v>
       </c>
       <c r="C80">
-        <v>129.3318292528596</v>
+        <v>129.33182925285959</v>
       </c>
       <c r="D80" s="2">
         <v>45839</v>
@@ -1734,7 +1772,7 @@
         <v>123.6165894780663</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>2025</v>
       </c>
@@ -1751,7 +1789,7 @@
         <v>123.6655045012229</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>2025</v>
       </c>
@@ -1768,7 +1806,7 @@
         <v>123.3126918873914</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>2025</v>
       </c>
@@ -1776,7 +1814,7 @@
         <v>10</v>
       </c>
       <c r="C83">
-        <v>129.5238590804855</v>
+        <v>129.52385908048549</v>
       </c>
       <c r="D83" s="2">
         <v>45931</v>
@@ -1785,7 +1823,7 @@
         <v>124.1619399490035</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>2025</v>
       </c>
@@ -1793,7 +1831,7 @@
         <v>11</v>
       </c>
       <c r="C84">
-        <v>129.9393556563299</v>
+        <v>129.93935565632989</v>
       </c>
       <c r="D84" s="2">
         <v>45962</v>
@@ -1802,7 +1840,7 @@
         <v>124.4023520840922</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>2025</v>
       </c>
@@ -1818,6 +1856,8 @@
       <c r="E85">
         <v>124.8290576052454</v>
       </c>
+      <c r="G85" s="3"/>
+      <c r="I85" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>